<commit_message>
changed 3 col headings
</commit_message>
<xml_diff>
--- a/churn_template.xlsx
+++ b/churn_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\Codebase\projects\Customer_churn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3065DB8A-225F-4DD9-AC25-6F52EF3FDE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2032FB1C-B6FC-4C78-9F5E-664287CC618C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>Dependents</t>
   </si>
   <si>
-    <t>tenure</t>
-  </si>
-  <si>
     <t>PhoneService</t>
   </si>
   <si>
@@ -73,12 +70,6 @@
     <t>PaperlessBilling</t>
   </si>
   <si>
-    <t>PaymentMethod</t>
-  </si>
-  <si>
-    <t>MonthlyCharges</t>
-  </si>
-  <si>
     <t>TotalCharges</t>
   </si>
   <si>
@@ -191,6 +182,15 @@
   </si>
   <si>
     <t>5129-JLPIS</t>
+  </si>
+  <si>
+    <t>MonthlyCharges(Rs.)</t>
+  </si>
+  <si>
+    <t>TotalCharges(Rs.)</t>
+  </si>
+  <si>
+    <t>tenure(months)</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,50 +616,50 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -667,55 +667,55 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <v>123</v>
       </c>
       <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
+      <c r="Q2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" t="s">
         <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" t="s">
-        <v>26</v>
       </c>
       <c r="S2">
         <v>123</v>
@@ -726,58 +726,58 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
         <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" t="s">
-        <v>34</v>
       </c>
       <c r="S3">
         <v>29.85</v>
@@ -788,58 +788,58 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F4">
         <v>34</v>
       </c>
       <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="S4">
         <v>56.95</v>
@@ -850,58 +850,58 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" t="s">
         <v>30</v>
       </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" t="s">
-        <v>33</v>
-      </c>
       <c r="Q5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="S5">
         <v>53.85</v>
@@ -912,58 +912,58 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F6">
         <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="S6">
         <v>42.3</v>
@@ -974,58 +974,58 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" t="s">
         <v>30</v>
       </c>
-      <c r="I7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N7" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" t="s">
-        <v>33</v>
-      </c>
       <c r="Q7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="S7">
         <v>70.7</v>
@@ -1036,58 +1036,58 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8">
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" t="s">
         <v>30</v>
       </c>
-      <c r="K8" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N8" t="s">
-        <v>29</v>
-      </c>
-      <c r="O8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" t="s">
-        <v>33</v>
-      </c>
       <c r="Q8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="S8">
         <v>99.65</v>
@@ -1098,58 +1098,58 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9">
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" t="s">
         <v>43</v>
-      </c>
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9" t="s">
-        <v>46</v>
       </c>
       <c r="S9">
         <v>89.1</v>
@@ -1160,58 +1160,58 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F10">
         <v>10</v>
       </c>
       <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" t="s">
         <v>30</v>
       </c>
-      <c r="H10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" t="s">
-        <v>30</v>
-      </c>
-      <c r="O10" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" t="s">
-        <v>33</v>
-      </c>
       <c r="Q10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="S10">
         <v>29.75</v>
@@ -1222,58 +1222,58 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F11">
         <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" t="s">
         <v>30</v>
       </c>
-      <c r="K11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" t="s">
-        <v>29</v>
-      </c>
-      <c r="M11" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" t="s">
-        <v>29</v>
-      </c>
-      <c r="O11" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11" t="s">
-        <v>33</v>
-      </c>
       <c r="Q11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="S11">
         <v>104.8</v>
@@ -1284,58 +1284,58 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F12">
         <v>62</v>
       </c>
       <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
         <v>29</v>
       </c>
-      <c r="H12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" t="s">
-        <v>32</v>
-      </c>
       <c r="J12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="S12">
         <v>56.15</v>
@@ -1346,58 +1346,58 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F13">
         <v>13</v>
       </c>
       <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" t="s">
         <v>29</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" t="s">
         <v>30</v>
       </c>
-      <c r="I13" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" t="s">
-        <v>29</v>
-      </c>
-      <c r="K13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" t="s">
-        <v>30</v>
-      </c>
-      <c r="M13" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" t="s">
-        <v>30</v>
-      </c>
-      <c r="O13" t="s">
-        <v>30</v>
-      </c>
-      <c r="P13" t="s">
-        <v>33</v>
-      </c>
       <c r="Q13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="S13">
         <v>49.95</v>
@@ -1408,58 +1408,58 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F14">
         <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="N14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="S14">
         <v>18.95</v>
@@ -1470,58 +1470,58 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F15">
         <v>58</v>
       </c>
       <c r="G15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R15" t="s">
         <v>43</v>
-      </c>
-      <c r="J15" t="s">
-        <v>30</v>
-      </c>
-      <c r="K15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" t="s">
-        <v>29</v>
-      </c>
-      <c r="M15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>30</v>
-      </c>
-      <c r="R15" t="s">
-        <v>46</v>
       </c>
       <c r="S15">
         <v>100.35</v>
@@ -1532,58 +1532,58 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F16">
         <v>49</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" t="s">
         <v>30</v>
       </c>
-      <c r="K16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M16" t="s">
-        <v>30</v>
-      </c>
-      <c r="N16" t="s">
-        <v>29</v>
-      </c>
-      <c r="O16" t="s">
-        <v>29</v>
-      </c>
-      <c r="P16" t="s">
-        <v>33</v>
-      </c>
       <c r="Q16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="S16">
         <v>103.7</v>
@@ -1594,58 +1594,58 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F17">
         <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" t="s">
         <v>30</v>
       </c>
-      <c r="I17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" t="s">
-        <v>29</v>
-      </c>
-      <c r="O17" t="s">
-        <v>29</v>
-      </c>
-      <c r="P17" t="s">
-        <v>33</v>
-      </c>
       <c r="Q17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="S17">
         <v>105.5</v>

</xml_diff>